<commit_message>
19.10.2024 - PART 1
</commit_message>
<xml_diff>
--- a/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST_REVISED.xlsx
+++ b/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST_REVISED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westhomas/Desktop/ALFRED/1__REPORT_AUTOMATION/REFERENCE_FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3047570F-0237-2647-96FC-4E54818D7555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15703F14-4F84-6B44-A01D-74E159E54028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" activeTab="1" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
   </bookViews>
@@ -20,8 +20,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId5"/>
-    <pivotCache cacheId="11" r:id="rId6"/>
+    <pivotCache cacheId="19" r:id="rId5"/>
+    <pivotCache cacheId="20" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>REFERECE</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Sum of FORMULA</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -147,6 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,9 +192,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wes Thomas" refreshedDate="45580.903931134257" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{12C083AD-9D31-A547-AD06-0A40DA36DECD}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wes Thomas" refreshedDate="45584.515307407404" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{59E39CD8-9BA5-6144-B26C-E4AF1FA91B09}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C2" sheet="INPUT_1"/>
+    <worksheetSource ref="A1:C3" sheet="INPUT_1"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="REFERECE" numFmtId="0">
@@ -199,7 +203,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="TEST_CELL" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="2"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="2">
+        <n v="2"/>
+        <n v="1"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="FORMULA" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="10"/>
@@ -223,17 +230,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
   <r>
     <x v="0"/>
-    <n v="2"/>
+    <x v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
     <n v="10"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ADABE3A-34B9-3044-8921-7AFEB81F8B06}" name="PT_1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ADABE3A-34B9-3044-8921-7AFEB81F8B06}" name="PT_1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -274,31 +286,48 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3F0C458-CA25-9E44-BBC9-4E47F3964C72}" name="PT_2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95499CBD-01A9-D443-94DF-F9004E1B1D57}" name="PT_2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
     <field x="0"/>
-  </rowFields>
-  <rowItems count="2">
+  </colFields>
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of FORMULA" fld="2" baseField="0" baseItem="0"/>
@@ -666,40 +695,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71603A94-795F-7644-BCD4-441D9E2BD689}">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="C5" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B6" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="C6" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>10</v>
+      <c r="B7" s="6">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -709,10 +767,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931970F3-AC3E-4630-A91D-2D0AC1BCB3ED}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,6 +811,18 @@
       </c>
       <c r="J2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>IF(A3&lt;&gt;B3,VLOOKUP(A3,INPUT_2!A:B,2,0),VLOOKUP(B3,INPUT_2!A:B,2,0))</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -827,15 +897,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006558401F0A96BE4BB0F9C1E3EB844901" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c79a549d573087af1da6ceb5b747f57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xmlns:ns4="da434bd8-e7d8-4f05-bd5c-7c1ec0b08732" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b00c1cc3168c7713bb0a38f65aaec641" ns3:_="" ns4:_="">
     <xsd:import namespace="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
@@ -1062,7 +1123,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xsi:nil="true"/>
@@ -1070,15 +1131,16 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E06FC62-AAD0-4BB6-8BAB-D339E38C5417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1097,7 +1159,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CF534CB-940E-49BD-9162-3839749B4EEF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1112,4 +1174,12 @@
     <ds:schemaRef ds:uri="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
27.10.2024 - PART 1
</commit_message>
<xml_diff>
--- a/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST_REVISED.xlsx
+++ b/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST_REVISED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westhomas/Desktop/ALFRED/1__REPORT_AUTOMATION/REFERENCE_FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15703F14-4F84-6B44-A01D-74E159E54028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BBB499-43E1-6747-8DAD-6C9F35E2325B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" activeTab="1" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
+    <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" activeTab="2" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
   </bookViews>
   <sheets>
     <sheet name="OUTPUT_1" sheetId="4" r:id="rId1"/>
@@ -18,10 +18,13 @@
     <sheet name="INPUT_1" sheetId="2" r:id="rId3"/>
     <sheet name="INPUT_2" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="TEST_RANGE">INPUT_1!$O$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId5"/>
-    <pivotCache cacheId="20" r:id="rId6"/>
+    <pivotCache cacheId="23" r:id="rId5"/>
+    <pivotCache cacheId="24" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -141,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -150,7 +153,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,7 +247,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ADABE3A-34B9-3044-8921-7AFEB81F8B06}" name="PT_1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ADABE3A-34B9-3044-8921-7AFEB81F8B06}" name="PT_1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -286,7 +288,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95499CBD-01A9-D443-94DF-F9004E1B1D57}" name="PT_2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95499CBD-01A9-D443-94DF-F9004E1B1D57}" name="PT_2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -655,7 +657,7 @@
   <dimension ref="A3:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -697,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71603A94-795F-7644-BCD4-441D9E2BD689}">
   <dimension ref="A3:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -731,10 +733,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>10</v>
       </c>
     </row>
@@ -742,10 +744,10 @@
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>10</v>
       </c>
     </row>
@@ -753,10 +755,10 @@
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>20</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>20</v>
       </c>
     </row>
@@ -767,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931970F3-AC3E-4630-A91D-2D0AC1BCB3ED}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -778,7 +780,7 @@
     <col min="10" max="10" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,8 +796,11 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="O1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -813,7 +818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1124,20 +1129,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,6 +1165,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CF534CB-940E-49BD-9162-3839749B4EEF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1174,12 +1187,4 @@
     <ds:schemaRef ds:uri="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>